<commit_message>
adding patch version of prevention, rehab and children
</commit_message>
<xml_diff>
--- a/children/StructureDefinition-BasedOnInterventionExtension.xlsx
+++ b/children/StructureDefinition-BasedOnInterventionExtension.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>2.0.0</t>
+    <t>2.0.1</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-06-05T11:21:47+02:00</t>
+    <t>2024-06-21T14:15:43+02:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
Revert "adding patch version of prevention, rehab and children"
This reverts commit 47da460be970f324dd040ef3559a058a035b752f.
</commit_message>
<xml_diff>
--- a/children/StructureDefinition-BasedOnInterventionExtension.xlsx
+++ b/children/StructureDefinition-BasedOnInterventionExtension.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>2.0.1</t>
+    <t>2.0.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-06-21T14:15:43+02:00</t>
+    <t>2024-06-05T11:21:47+02:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
adding children 2.1.0, rehab 2.2.0 and kl-gateway 1.2.0
</commit_message>
<xml_diff>
--- a/children/StructureDefinition-BasedOnInterventionExtension.xlsx
+++ b/children/StructureDefinition-BasedOnInterventionExtension.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>2.0.1</t>
+    <t>2.1.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-07-01T22:52:03+02:00</t>
+    <t>2024-10-31T20:37:15+01:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>